<commit_message>
Agregar contenido en las tablas de QA para el registro de usuario
</commit_message>
<xml_diff>
--- a/qa/test-data/usuarios.xlsx
+++ b/qa/test-data/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\busin\PocketCloset\qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FD4177-62F8-43EF-BBAE-67E7D92C9B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A029E289-6937-46D7-B0F3-92F442A3DEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -892,9 +892,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -937,6 +934,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,10 +952,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1264,571 +1260,571 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+      <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="9" t="s">
+      <c r="D16" s="23"/>
+      <c r="E16" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="17">
+      <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
+      <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="17">
+      <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="17">
+      <c r="A23" s="16">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="17">
+      <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="18">
+      <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1854,210 +1850,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="31">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="31">
+      <c r="A3" s="30">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="31">
+      <c r="A4" s="30">
         <v>3</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="31">
+      <c r="A5" s="30">
         <v>4</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="31">
+      <c r="A6" s="30">
         <v>5</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="31">
+      <c r="A7" s="30">
         <v>6</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="31">
+      <c r="A8" s="30">
         <v>7</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="31">
+      <c r="A9" s="30">
         <v>8</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
+      <c r="A10" s="30">
         <v>9</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="31">
+      <c r="A11" s="30">
         <v>10</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="31">
+      <c r="A12" s="30">
         <v>11</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="31">
+      <c r="A13" s="30">
         <v>12</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="31">
+      <c r="A14" s="30">
         <v>13</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="31">
+      <c r="A15" s="30">
         <v>14</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="31">
+      <c r="A16" s="30">
         <v>15</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="31">
+      <c r="A17" s="30">
         <v>16</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="31">
+      <c r="A18" s="30">
         <v>17</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="31">
+      <c r="A19" s="30">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="31">
+      <c r="A20" s="30">
         <v>19</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="31">
+      <c r="A21" s="30">
         <v>20</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="31">
+      <c r="A22" s="30">
         <v>21</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="31">
+      <c r="A23" s="30">
         <v>22</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="31">
+      <c r="A24" s="30">
         <v>23</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="31">
+      <c r="A25" s="30">
         <v>24</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2069,7 +2065,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2087,58 +2083,58 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>